<commit_message>
Final commit ao original project
</commit_message>
<xml_diff>
--- a/com.Education.SMS/src/test/resources/TestData1.xlsx
+++ b/com.Education.SMS/src/test/resources/TestData1.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="258">
   <si>
     <t>TC_ID</t>
   </si>
@@ -208,12 +208,599 @@
   </si>
   <si>
     <t>full_name</t>
+  </si>
+  <si>
+    <t>Afghanistan</t>
+  </si>
+  <si>
+    <t>Albania</t>
+  </si>
+  <si>
+    <t>Algeria</t>
+  </si>
+  <si>
+    <t>Andorra</t>
+  </si>
+  <si>
+    <t>Angola</t>
+  </si>
+  <si>
+    <t>Antigua &amp; Barbuda</t>
+  </si>
+  <si>
+    <t>Argentina</t>
+  </si>
+  <si>
+    <t>Armenia</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>Austria</t>
+  </si>
+  <si>
+    <t>Azerbaijan</t>
+  </si>
+  <si>
+    <t>The Bahamas</t>
+  </si>
+  <si>
+    <t>Bahrain</t>
+  </si>
+  <si>
+    <t>Bangladesh</t>
+  </si>
+  <si>
+    <t>Barbados</t>
+  </si>
+  <si>
+    <t>Belarus</t>
+  </si>
+  <si>
+    <t>Belgium</t>
+  </si>
+  <si>
+    <t>Belize</t>
+  </si>
+  <si>
+    <t>Benin</t>
+  </si>
+  <si>
+    <t>Bhutan</t>
+  </si>
+  <si>
+    <t>Bolivia</t>
+  </si>
+  <si>
+    <t>Bosnia and Herzegovina</t>
+  </si>
+  <si>
+    <t>Botswana</t>
+  </si>
+  <si>
+    <t>Brazil</t>
+  </si>
+  <si>
+    <t>Brunei</t>
+  </si>
+  <si>
+    <t>Bulgaria</t>
+  </si>
+  <si>
+    <t>Burkina Faso</t>
+  </si>
+  <si>
+    <t>Burundi</t>
+  </si>
+  <si>
+    <t>Cambodia</t>
+  </si>
+  <si>
+    <t>Cameroon</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>Cape Verde</t>
+  </si>
+  <si>
+    <t>Central African Republic</t>
+  </si>
+  <si>
+    <t>Chad</t>
+  </si>
+  <si>
+    <t>Chile</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>Colombia</t>
+  </si>
+  <si>
+    <t>Comoros</t>
+  </si>
+  <si>
+    <t>Democratic Republic Of the Congo</t>
+  </si>
+  <si>
+    <t>Republic of the Congo</t>
+  </si>
+  <si>
+    <t>Costa Rica</t>
+  </si>
+  <si>
+    <t>Cote d’Ivoire (Ivory Coast)</t>
+  </si>
+  <si>
+    <t>Croatia</t>
+  </si>
+  <si>
+    <t>Cuba</t>
+  </si>
+  <si>
+    <t>Cyprus</t>
+  </si>
+  <si>
+    <t>Czechia</t>
+  </si>
+  <si>
+    <t>Denmark</t>
+  </si>
+  <si>
+    <t>Djibouti</t>
+  </si>
+  <si>
+    <t>Dominica</t>
+  </si>
+  <si>
+    <t>Dominican Republic</t>
+  </si>
+  <si>
+    <t>East Timor (Timor-Leste)</t>
+  </si>
+  <si>
+    <t>Ecuador</t>
+  </si>
+  <si>
+    <t>Egypt</t>
+  </si>
+  <si>
+    <t>El Salvador</t>
+  </si>
+  <si>
+    <t>Equitorial Guinea</t>
+  </si>
+  <si>
+    <t>Eritrea</t>
+  </si>
+  <si>
+    <t>Estonia</t>
+  </si>
+  <si>
+    <t>Ethiopia</t>
+  </si>
+  <si>
+    <t>Fiji</t>
+  </si>
+  <si>
+    <t>Finland</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>Gabon</t>
+  </si>
+  <si>
+    <t>The Gambia</t>
+  </si>
+  <si>
+    <t>Georgia</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>Ghana</t>
+  </si>
+  <si>
+    <t>Greece</t>
+  </si>
+  <si>
+    <t>Grenada</t>
+  </si>
+  <si>
+    <t>Guatemala</t>
+  </si>
+  <si>
+    <t>Guinea</t>
+  </si>
+  <si>
+    <t>Guinea-Bissau</t>
+  </si>
+  <si>
+    <t>Guyana</t>
+  </si>
+  <si>
+    <t>Haiti</t>
+  </si>
+  <si>
+    <t>Honduras</t>
+  </si>
+  <si>
+    <t>Hungary</t>
+  </si>
+  <si>
+    <t>Iceland</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Indonesia</t>
+  </si>
+  <si>
+    <t>Iran</t>
+  </si>
+  <si>
+    <t>Iraq</t>
+  </si>
+  <si>
+    <t>Republic of Ireland</t>
+  </si>
+  <si>
+    <t>Israel</t>
+  </si>
+  <si>
+    <t>Italy</t>
+  </si>
+  <si>
+    <t>Jamaica</t>
+  </si>
+  <si>
+    <t>Japan</t>
+  </si>
+  <si>
+    <t>Jordan</t>
+  </si>
+  <si>
+    <t>Kazakhstan</t>
+  </si>
+  <si>
+    <t>Kenya</t>
+  </si>
+  <si>
+    <t>Kiribati</t>
+  </si>
+  <si>
+    <t>North Korea</t>
+  </si>
+  <si>
+    <t>South Korea</t>
+  </si>
+  <si>
+    <t>Kosovo</t>
+  </si>
+  <si>
+    <t>Kuwait</t>
+  </si>
+  <si>
+    <t>Kyrgyzstan</t>
+  </si>
+  <si>
+    <t>Laos</t>
+  </si>
+  <si>
+    <t>Latvia</t>
+  </si>
+  <si>
+    <t>Lebanon</t>
+  </si>
+  <si>
+    <t>Lesotho</t>
+  </si>
+  <si>
+    <t>Liberia</t>
+  </si>
+  <si>
+    <t>Libya</t>
+  </si>
+  <si>
+    <t>Liechtenstein</t>
+  </si>
+  <si>
+    <t>Lithuania</t>
+  </si>
+  <si>
+    <t>Luxembourg</t>
+  </si>
+  <si>
+    <t>Macedonia</t>
+  </si>
+  <si>
+    <t>Madagascar</t>
+  </si>
+  <si>
+    <t>Malawi</t>
+  </si>
+  <si>
+    <t>Malaysia</t>
+  </si>
+  <si>
+    <t>Maldives</t>
+  </si>
+  <si>
+    <t>Mali</t>
+  </si>
+  <si>
+    <t>Malta</t>
+  </si>
+  <si>
+    <t>Marshall Islands</t>
+  </si>
+  <si>
+    <t>Mauritania</t>
+  </si>
+  <si>
+    <t>Mauritius</t>
+  </si>
+  <si>
+    <t>Mexico</t>
+  </si>
+  <si>
+    <t>Federal States of Micronesia</t>
+  </si>
+  <si>
+    <t>Moldova</t>
+  </si>
+  <si>
+    <t>Monaco</t>
+  </si>
+  <si>
+    <t>Mongolia</t>
+  </si>
+  <si>
+    <t>Montenegro</t>
+  </si>
+  <si>
+    <t>Morocco</t>
+  </si>
+  <si>
+    <t>Mozambique</t>
+  </si>
+  <si>
+    <t>Myanmar (Burma)</t>
+  </si>
+  <si>
+    <t>Namibia</t>
+  </si>
+  <si>
+    <t>Nauru</t>
+  </si>
+  <si>
+    <t>Nepal</t>
+  </si>
+  <si>
+    <t>Netherlands</t>
+  </si>
+  <si>
+    <t>New Zealand</t>
+  </si>
+  <si>
+    <t>Nicaragua</t>
+  </si>
+  <si>
+    <t>Niger</t>
+  </si>
+  <si>
+    <t>Nigeria</t>
+  </si>
+  <si>
+    <t>Norway</t>
+  </si>
+  <si>
+    <t>Oman</t>
+  </si>
+  <si>
+    <t>Pakistan</t>
+  </si>
+  <si>
+    <t>Palau</t>
+  </si>
+  <si>
+    <t>Panama</t>
+  </si>
+  <si>
+    <t>Papa New Guinea</t>
+  </si>
+  <si>
+    <t>Paraguay</t>
+  </si>
+  <si>
+    <t>Peru</t>
+  </si>
+  <si>
+    <t>Phillipines</t>
+  </si>
+  <si>
+    <t>Poland</t>
+  </si>
+  <si>
+    <t>Portugal</t>
+  </si>
+  <si>
+    <t>Qatar</t>
+  </si>
+  <si>
+    <t>Romania</t>
+  </si>
+  <si>
+    <t>Russia</t>
+  </si>
+  <si>
+    <t>Rwanda</t>
+  </si>
+  <si>
+    <t>Saint Kitts and Nevis</t>
+  </si>
+  <si>
+    <t>Saint Lucia</t>
+  </si>
+  <si>
+    <t>Saint Vincent and
+The Grenadines</t>
+  </si>
+  <si>
+    <t>Samoa</t>
+  </si>
+  <si>
+    <t>San Marino</t>
+  </si>
+  <si>
+    <t>Sao Tome and Principe</t>
+  </si>
+  <si>
+    <t>Saudi Arabia</t>
+  </si>
+  <si>
+    <t>Senegal</t>
+  </si>
+  <si>
+    <t>Serbia</t>
+  </si>
+  <si>
+    <t>Seychelles</t>
+  </si>
+  <si>
+    <t>Sierra Leone</t>
+  </si>
+  <si>
+    <t>Singapore</t>
+  </si>
+  <si>
+    <t>Slovakia</t>
+  </si>
+  <si>
+    <t>Slovenia</t>
+  </si>
+  <si>
+    <t>Solomon Islands</t>
+  </si>
+  <si>
+    <t>Somalia</t>
+  </si>
+  <si>
+    <t>South Africa</t>
+  </si>
+  <si>
+    <t>Spain</t>
+  </si>
+  <si>
+    <t>Sri Lanka</t>
+  </si>
+  <si>
+    <t>Sudan</t>
+  </si>
+  <si>
+    <t>Suriname</t>
+  </si>
+  <si>
+    <t>Swaziland</t>
+  </si>
+  <si>
+    <t>Sweden</t>
+  </si>
+  <si>
+    <t>Switzerland</t>
+  </si>
+  <si>
+    <t>Syria</t>
+  </si>
+  <si>
+    <t>Taiwan</t>
+  </si>
+  <si>
+    <t>Tajikistan</t>
+  </si>
+  <si>
+    <t>Tanzania</t>
+  </si>
+  <si>
+    <t>Thailand</t>
+  </si>
+  <si>
+    <t>Togo</t>
+  </si>
+  <si>
+    <t>Tonga</t>
+  </si>
+  <si>
+    <t>Trinidad and Tobago</t>
+  </si>
+  <si>
+    <t>Tunisia</t>
+  </si>
+  <si>
+    <t>Turkey</t>
+  </si>
+  <si>
+    <t>Turkmenistan</t>
+  </si>
+  <si>
+    <t>Tuvalu</t>
+  </si>
+  <si>
+    <t>Uganda</t>
+  </si>
+  <si>
+    <t>Ukraine</t>
+  </si>
+  <si>
+    <t>United Arab Emirates</t>
+  </si>
+  <si>
+    <t>United Kingdom</t>
+  </si>
+  <si>
+    <t>United States of America</t>
+  </si>
+  <si>
+    <t>Uruguay</t>
+  </si>
+  <si>
+    <t>Uzbekistan</t>
+  </si>
+  <si>
+    <t>Vanuatu</t>
+  </si>
+  <si>
+    <t>Vatican City</t>
+  </si>
+  <si>
+    <t>Venezuela</t>
+  </si>
+  <si>
+    <t>Vietnam</t>
+  </si>
+  <si>
+    <t>Yemen</t>
+  </si>
+  <si>
+    <t>Zambia</t>
+  </si>
+  <si>
+    <t>Zimbabwe</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -588,24 +1175,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" customWidth="1"/>
-    <col min="4" max="5" width="18.85546875" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" customWidth="1"/>
-    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.7109375" customWidth="1"/>
-    <col min="14" max="14" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="15.5703125"/>
+    <col min="3" max="3" customWidth="true" width="19.7109375"/>
+    <col min="4" max="5" customWidth="true" width="18.85546875"/>
+    <col min="6" max="6" customWidth="true" width="13.140625"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="11.0"/>
+    <col min="13" max="13" customWidth="true" width="18.7109375"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="13.28515625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
+    <row r="1">
+      <c r="B1" t="s" s="0">
+        <v>257</v>
       </c>
     </row>
     <row r="2" spans="1:14">
@@ -618,7 +1199,7 @@
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" t="s" s="0">
         <v>13</v>
       </c>
     </row>
@@ -661,37 +1242,37 @@
       </c>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4">
+      <c r="A4" s="0">
         <v>144</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" t="s" s="0">
         <v>7</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="0">
         <v>2255889966</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" t="s" s="0">
         <v>18</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="M4" t="s">
+      <c r="M4" t="s" s="0">
         <v>21</v>
       </c>
       <c r="N4" s="4" t="s">
@@ -716,7 +1297,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>35</v>
       </c>
     </row>
@@ -735,16 +1316,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
-    <col min="2" max="2" width="23" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" customWidth="1"/>
-    <col min="5" max="6" width="17.7109375" customWidth="1"/>
-    <col min="7" max="7" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="22.42578125"/>
+    <col min="2" max="2" customWidth="true" width="23.0"/>
+    <col min="3" max="3" customWidth="true" width="16.7109375"/>
+    <col min="4" max="4" customWidth="true" width="17.85546875"/>
+    <col min="5" max="6" customWidth="true" width="17.7109375"/>
+    <col min="7" max="7" customWidth="true" width="18.42578125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>24</v>
       </c>
     </row>
@@ -772,22 +1353,22 @@
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3">
+      <c r="A3" s="0">
         <v>10000000055</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>31</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>32</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>33</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" t="s" s="0">
         <v>7</v>
       </c>
       <c r="G3" s="5" t="s">
@@ -813,11 +1394,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" customWidth="1"/>
-    <col min="3" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="19" customWidth="1"/>
-    <col min="6" max="6" width="18.85546875" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="17.5703125"/>
+    <col min="2" max="2" customWidth="true" width="14.5703125"/>
+    <col min="3" max="4" customWidth="true" width="18.0"/>
+    <col min="5" max="5" customWidth="true" width="19.0"/>
+    <col min="6" max="6" customWidth="true" width="18.85546875"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:6">
@@ -841,19 +1422,19 @@
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>40</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>41</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>36</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" t="s" s="0">
         <v>38</v>
       </c>
       <c r="F3" s="5" t="s">
@@ -879,10 +1460,10 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>33</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>44</v>
       </c>
       <c r="C1" s="6" t="s">
@@ -890,10 +1471,10 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>45</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>46</v>
       </c>
       <c r="C2" s="6" t="s">
@@ -901,10 +1482,10 @@
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>47</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>48</v>
       </c>
       <c r="C3" s="6" t="s">
@@ -926,8 +1507,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" customWidth="1"/>
-    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="23.85546875"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="18.0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -939,10 +1520,10 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>62</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>56</v>
       </c>
     </row>
@@ -950,7 +1531,7 @@
       <c r="A3" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>57</v>
       </c>
     </row>
@@ -958,7 +1539,7 @@
       <c r="A4" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>58</v>
       </c>
     </row>
@@ -966,7 +1547,7 @@
       <c r="A5" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>59</v>
       </c>
     </row>

</xml_diff>